<commit_message>
Added More Utility Functions
</commit_message>
<xml_diff>
--- a/Baseline_Oxy_FoodDep_BoostAndEtho_Ghrelin_Saline_Cluster_Tables/Baseline DT_1.xlsx
+++ b/Baseline_Oxy_FoodDep_BoostAndEtho_Ghrelin_Saline_Cluster_Tables/Baseline DT_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ddc81097063262a/Desktop/ghrelin_paper/Baseline_Oxy_FoodDep_BoostAndEtho_Ghrelin_Saline_Cluster_Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_514D4DEFC80EAF6EA6745F44E5012D16118A2732" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_514D4DEFC80EAF6EA6745F44E5012D16118A2732" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA04EBC-16F7-466B-92FE-81DE9B337BB1}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -671,14 +671,14 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
updated to correct directory name
</commit_message>
<xml_diff>
--- a/Baseline_Oxy_FoodDep_BoostAndEtho_Ghrelin_Saline_Cluster_Tables/Baseline DT_1.xlsx
+++ b/Baseline_Oxy_FoodDep_BoostAndEtho_Ghrelin_Saline_Cluster_Tables/Baseline DT_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="11_514D4DEFC80EAF6EA6745F44E5012D16118A2732" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EA04EBC-16F7-466B-92FE-81DE9B337BB1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -369,6 +369,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -671,7 +675,7 @@
   <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>